<commit_message>
1. Created Xml files 2. Created suite xml files and executed in the group
</commit_message>
<xml_diff>
--- a/src/test/java/com/shopclues/testdata/home.xlsx
+++ b/src/test/java/com/shopclues/testdata/home.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1695" windowWidth="15375" windowHeight="7875" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15960" windowHeight="2595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Registration" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -53,40 +54,19 @@
     <t>basheer@test.com</t>
   </si>
   <si>
-    <t>selenium</t>
-  </si>
-  <si>
-    <t>Abhijith</t>
-  </si>
-  <si>
     <t>selenium@admin.com</t>
   </si>
   <si>
     <t>test8765@gmail.com</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>test1234</t>
-  </si>
-  <si>
-    <t>selenium1234</t>
-  </si>
-  <si>
-    <t>java9876</t>
-  </si>
-  <si>
-    <t>BBBBB</t>
-  </si>
-  <si>
-    <t>SSSSS</t>
-  </si>
-  <si>
-    <t>AAAAA</t>
+    <t>5555555555</t>
+  </si>
+  <si>
+    <t>66666666</t>
+  </si>
+  <si>
+    <t>777777777</t>
   </si>
 </sst>
 </file>
@@ -160,11 +140,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,13 +432,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -498,81 +481,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>